<commit_message>
Env parameters and inter round variation added to the code
</commit_message>
<xml_diff>
--- a/clean_file.xlsx
+++ b/clean_file.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,17 +423,19 @@
   <cols>
     <col width="18" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="13" customWidth="1" min="3" max="3"/>
     <col width="7" customWidth="1" min="4" max="4"/>
-    <col width="56" customWidth="1" min="5" max="5"/>
-    <col width="80" customWidth="1" min="6" max="6"/>
-    <col width="32" customWidth="1" min="7" max="7"/>
-    <col width="154" customWidth="1" min="8" max="8"/>
-    <col width="16" customWidth="1" min="9" max="9"/>
-    <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="10" customWidth="1" min="11" max="11"/>
-    <col width="660" customWidth="1" min="12" max="12"/>
-    <col width="35" customWidth="1" min="13" max="13"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
+    <col width="29" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="7" max="7"/>
+    <col width="8" customWidth="1" min="8" max="8"/>
+    <col width="19" customWidth="1" min="9" max="9"/>
+    <col width="66" customWidth="1" min="10" max="10"/>
+    <col width="16" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="317" customWidth="1" min="14" max="14"/>
+    <col width="19" customWidth="1" min="15" max="15"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -474,30 +476,40 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>Vround</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Score_reel_flower</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
           <t>Noise_applied</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Total_earnings</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>Birth_year</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>Feedback</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>QCM_sequence_raw</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>QCM_sequence_bool</t>
         </is>
@@ -506,7 +518,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>hyjpk071</t>
+          <t>ya5c2ooh</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -541,31 +553,41 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>["3", "3"]</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
           <t>[null, null]</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>0.06</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>[{"slide":"5/9","text":"Earnings are determined randomly","correct":false,"timestamp":1767699023568},{"slide":"5/9","text":"How fast I choose the configurations","correct":false,"timestamp":1767699024218},{"slide":"5/9","text":"Flower growth based on my nutrient choices","correct":true,"timestamp":1767699025137},{"slide":"8/9","text":"Your final payoff is calculated by adding the earnings from each round.","correct":false,"timestamp":1767699031031},{"slide":"8/9","text":"Your final payoff is calculated by adding the earnings from each round, plus the earnings of the  two tests added to the total at the end.","correct":true,"timestamp":1767699031834}]</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>[False, False, True, False, True]</t>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>[{"slide":"5/9","text":"Flower growth based on my nutrient choices","correct":true,"timestamp":1768993827630},{"slide":"8/9","text":"Your final payoff is calculated by adding the earnings from each round, plus the earnings of the  two tests added to the total at the end.","correct":true,"timestamp":1768993829629}]</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>[True, True]</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>hyjpk071</t>
+          <t>ya5c2ooh</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -600,18 +622,28 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>["4", "4"]</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
           <t>[null, null]</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>0.12</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0.14</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr">
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -620,53 +652,31 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>hyjpk071</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Anomaly no noise</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>First phase</t>
-        </is>
-      </c>
+          <t>ya5c2ooh</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>["Purple", "Green", "Green"]</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>[["Red", ""], ["Red", ""], ["Red", ""]]</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>[0.3, 0.3, 0.3]</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>[null, null, null]</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>0.21</t>
-        </is>
-      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>0.14</t>
+        </is>
+      </c>
       <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr">
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -675,53 +685,31 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>hyjpk071</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Anomaly no noise</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>First phase</t>
-        </is>
-      </c>
+          <t>ya5c2ooh</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>["Green", "Purple", "Purple"]</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>[["Red", ""], ["Red", ""], ["Red", ""]]</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>[0.3, 0.3, 0.3]</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>[null, null, null]</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>0.3</t>
-        </is>
-      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr">
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -730,53 +718,31 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>hyjpk071</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Anomaly no noise</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Test 1</t>
-        </is>
-      </c>
+          <t>ya5c2ooh</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>["Green", "Yellow", "Purple", "Red", "Orange", "Blue"]</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>[["Red", ""], ["Red", ""], ["Red", ""], ["Red", ""], ["Red", ""], ["Red", ""]]</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>[0.6, 0.6, 0.6, 0.6, 0.6, 0.6]</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>[null, null, null, null, null, null]</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>0.3</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr">
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -785,53 +751,31 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>hyjpk071</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Anomaly no noise</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Second phase</t>
-        </is>
-      </c>
+          <t>ya5c2ooh</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>["Orange", "Purple"]</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>[["Red", ""], ["Red", ""]]</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>[0.3, 0.3]</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>[null, null]</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>0.36</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr">
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -840,53 +784,31 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>hyjpk071</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Anomaly no noise</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Second phase</t>
-        </is>
-      </c>
+          <t>ya5c2ooh</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>["Orange", "Green"]</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>[["Red", ""], ["Red", ""]]</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>[0.3, 0.3]</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>[null, null]</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>0.42</t>
-        </is>
-      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
       <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr">
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -895,53 +817,31 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>hyjpk071</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Anomaly no noise</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Second phase</t>
-        </is>
-      </c>
+          <t>ya5c2ooh</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>["Green", "Red", "Green"]</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>[["Red", ""], ["Red", ""], ["Red", ""]]</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>[0.3, 0.3, 0.3]</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>[null, null, null]</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>0.51</t>
-        </is>
-      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
       <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr">
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -950,53 +850,31 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>hyjpk071</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Anomaly no noise</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Second phase</t>
-        </is>
-      </c>
+          <t>ya5c2ooh</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>["Blue", "Purple", "Purple"]</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>[["Red", ""], ["Red", ""], ["Red", ""]]</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>[0.3, 0.3, 0.3]</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>[null, null, null]</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>0.6</t>
-        </is>
-      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
       <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr">
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -1005,53 +883,31 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>hyjpk071</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Anomaly no noise</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Second phase</t>
-        </is>
-      </c>
+          <t>ya5c2ooh</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>["Purple", "Green", "Yellow"]</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>[["Red", ""], ["Red", ""], ["Red", ""]]</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>[0.3, 0.3, 0.3]</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>[null, null, null]</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>0.69</t>
-        </is>
-      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
       <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr">
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -1060,53 +916,31 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>hyjpk071</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Anomaly no noise</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Test 2</t>
-        </is>
-      </c>
+          <t>ya5c2ooh</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>["Green", "Yellow", "Purple", "Red", "Orange", "Blue"]</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>[["Red", ""], ["Red", ""], ["Red", ""], ["Red", ""], ["Red", ""], ["Red", ""]]</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>[0.6, 0.6, 0.6, 0.6, 0.6, 0.6]</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>[null, null, null, null, null, null]</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>1.41</t>
-        </is>
-      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
       <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr">
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -1115,158 +949,198 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>hyjpk071</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Anomaly no noise</t>
-        </is>
-      </c>
+          <t>ya5c2ooh</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Results</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>1.41</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>2019</t>
-        </is>
-      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Annaa</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>n6nopx8w</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>No Anomaly noisy</t>
-        </is>
-      </c>
+          <t>ya5c2ooh</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>First phase</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>["Purple", "Green"]</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>[["Red", ""], ["Red", ""]]</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>[0.3, 0.5]</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>[{"index": 0, "type": "none", "amount": 0.0, "before": 0.3, "after": 0.3}, {"index": 1, "type": "increase", "amount": 0.2, "before": 0.3, "after": 0.5}]</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>0.08</t>
-        </is>
-      </c>
+          <t>Results</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>[{"slide":"5/9","text":"Earnings are determined randomly","correct":false,"timestamp":1767699517478},{"slide":"5/9","text":"How fast I choose the configurations","correct":false,"timestamp":1767699518490},{"slide":"5/9","text":"Flower growth based on my nutrient choices","correct":true,"timestamp":1767699519155},{"slide":"8/9","text":"Your final payoff is calculated by adding the earnings from each round, plus the earnings of the  two tests added to the total at the end.","correct":true,"timestamp":1767699524342}]</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>[False, False, True, True]</t>
-        </is>
-      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>n6nopx8w</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
+          <t>sfsaqxt0</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Anomaly noisy</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>First phase</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>["Purple", "Green"]</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>[["Red", ""], ["Red", ""]]</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>[0.3, 0.3]</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="I15" t="inlineStr">
         <is>
+          <t>["5", "3"]</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>[{"index": 0, "type": "increase"}, {"index": 1, "type": "none"}]</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
           <t>0.08</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>[]</t>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>[{"slide":"5/9","text":"Flower growth based on my nutrient choices","correct":true,"timestamp":1768993815884},{"slide":"8/9","text":"Your final payoff is calculated by adding the earnings from each round, plus the earnings of the  two tests added to the total at the end.","correct":true,"timestamp":1768993817791}]</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>[True, True]</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>n6nopx8w</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
+          <t>sfsaqxt0</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Anomaly noisy</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>First phase</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>["Green", "Purple"]</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>[["Blue", ""], ["Red", ""]]</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>[0.5, 0.3]</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
+          <t>["8", "4"]</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>[{"index": 0, "type": "increase"}, {"index": 1, "type": "none"}]</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
       <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr">
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -1275,29 +1149,31 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>n6nopx8w</t>
+          <t>sfsaqxt0</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
       <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr">
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -1306,29 +1182,31 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>n6nopx8w</t>
+          <t>sfsaqxt0</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
       <c r="L18" t="inlineStr"/>
-      <c r="M18" t="inlineStr">
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -1337,29 +1215,31 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>n6nopx8w</t>
+          <t>sfsaqxt0</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
       <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr">
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -1368,29 +1248,31 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>n6nopx8w</t>
+          <t>sfsaqxt0</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
       <c r="L20" t="inlineStr"/>
-      <c r="M20" t="inlineStr">
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -1399,29 +1281,31 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>n6nopx8w</t>
+          <t>sfsaqxt0</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
       <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr">
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -1430,29 +1314,31 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>n6nopx8w</t>
+          <t>sfsaqxt0</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr"/>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
       <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr">
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -1461,29 +1347,31 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>n6nopx8w</t>
+          <t>sfsaqxt0</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
       <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr">
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -1492,33 +1380,31 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>n6nopx8w</t>
+          <t>sfsaqxt0</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Test 2</t>
-        </is>
-      </c>
+      <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
       <c r="L24" t="inlineStr"/>
-      <c r="M24" t="inlineStr">
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -1527,29 +1413,101 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>n6nopx8w</t>
+          <t>sfsaqxt0</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Results</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
+      <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr"/>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
       <c r="L25" t="inlineStr"/>
       <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>sfsaqxt0</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Test 2</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>sfsaqxt0</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Results</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>